<commit_message>
More Queries and another script
Added a new script and a few more queries to sql folder
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Desktop\pollitt-master - Copy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Desktop\Data_mining_w_pollitt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -374,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3390,6 +3390,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>197</v>
+      </c>
+      <c r="B87">
+        <v>7</v>
+      </c>
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87">
+        <v>5</v>
+      </c>
+      <c r="F87">
+        <v>7</v>
+      </c>
+      <c r="G87">
+        <v>7</v>
+      </c>
+      <c r="H87">
+        <v>6</v>
+      </c>
+      <c r="I87">
+        <v>5</v>
+      </c>
+      <c r="J87">
+        <v>4</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>